<commit_message>
Added comments & updated spreadsheet
</commit_message>
<xml_diff>
--- a/data/ClueLayout.xlsx
+++ b/data/ClueLayout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Java\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Waite\Downloads\C13A-1_Waite_Day\C13A-1_Waite_Day\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0569D685-A6BD-46B7-9AB0-38E7B98EFC9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B7D0C4D-C32C-44F0-9BC5-FB9E44682106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5955" xr2:uid="{C96ABDD4-057B-46D0-A104-E68A1331A738}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C96ABDD4-057B-46D0-A104-E68A1331A738}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="42">
   <si>
     <t>X</t>
   </si>
@@ -136,6 +136,21 @@
   </si>
   <si>
     <t>H*</t>
+  </si>
+  <si>
+    <t>White:  Door Direction Tests (FileInitTest)</t>
+  </si>
+  <si>
+    <t>Light Orange: Room/Door Adjacency Tests</t>
+  </si>
+  <si>
+    <t>Dark Orange: Walkway Adjacency Tests</t>
+  </si>
+  <si>
+    <t>Light Blue: Target Tests</t>
+  </si>
+  <si>
+    <t>Red: Test Occupied</t>
   </si>
 </sst>
 </file>
@@ -159,7 +174,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -196,6 +211,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -209,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -227,6 +272,25 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -543,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EA1485F-C08E-42B3-AE09-AA6D557C99D0}">
-  <dimension ref="A1:Z30"/>
+  <dimension ref="A1:AH30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="W16" activeCellId="1" sqref="X21 W16"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,7 +619,7 @@
     <col min="2" max="26" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4">
         <v>0</v>
@@ -633,11 +697,11 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -652,7 +716,7 @@
       <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="13" t="s">
         <v>14</v>
       </c>
       <c r="H2" s="3" t="s">
@@ -691,7 +755,7 @@
       <c r="S2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="T2" s="11" t="s">
         <v>14</v>
       </c>
       <c r="U2" s="6" t="s">
@@ -712,8 +776,11 @@
       <c r="Z2" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="AB2" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -793,7 +860,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -833,7 +900,7 @@
       <c r="M4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="13" t="s">
         <v>30</v>
       </c>
       <c r="O4" s="1" t="s">
@@ -872,8 +939,16 @@
       <c r="Z4" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="AB4" s="7"/>
+      <c r="AD4" s="8"/>
+      <c r="AE4" s="8"/>
+      <c r="AF4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="AG4" s="8"/>
+      <c r="AH4" s="8"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -952,8 +1027,14 @@
       <c r="Z5" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="AD5" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE5" s="10"/>
+      <c r="AF5" s="10"/>
+      <c r="AG5" s="10"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -1029,11 +1110,16 @@
       <c r="Y6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="Z6" s="6" t="s">
-        <v>14</v>
-      </c>
+      <c r="Z6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD6" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE6" s="12"/>
+      <c r="AF6" s="12"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -1064,7 +1150,7 @@
       <c r="J7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="K7" s="15" t="s">
         <v>14</v>
       </c>
       <c r="L7" s="6" t="s">
@@ -1112,8 +1198,12 @@
       <c r="Z7" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="AD7" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE7" s="14"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -1193,7 +1283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -1273,14 +1363,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>8</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="5" t="s">
+      <c r="B10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D10" s="6" t="s">
@@ -1353,7 +1443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -1433,7 +1523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -1513,7 +1603,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -1593,7 +1683,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -1673,7 +1763,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -1701,7 +1791,7 @@
       <c r="I15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="J15" s="9" t="s">
         <v>18</v>
       </c>
       <c r="K15" s="6" t="s">
@@ -1728,7 +1818,7 @@
       <c r="R15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="S15" s="6" t="s">
+      <c r="S15" s="13" t="s">
         <v>14</v>
       </c>
       <c r="T15" s="6" t="s">
@@ -1753,7 +1843,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -1837,7 +1927,7 @@
       <c r="A17" s="4">
         <v>15</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="13" t="s">
         <v>22</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -2131,7 +2221,7 @@
       <c r="S20" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="T20" s="5" t="s">
+      <c r="T20" s="7" t="s">
         <v>16</v>
       </c>
       <c r="U20" s="1" t="s">
@@ -2166,7 +2256,7 @@
       <c r="D21" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="11" t="s">
         <v>14</v>
       </c>
       <c r="F21" s="6" t="s">
@@ -2208,10 +2298,10 @@
       <c r="R21" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="S21" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="T21" s="5" t="s">
+      <c r="S21" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="T21" s="15" t="s">
         <v>16</v>
       </c>
       <c r="U21" s="1" t="s">
@@ -2273,7 +2363,7 @@
       <c r="M22" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="N22" s="5" t="s">
+      <c r="N22" s="7" t="s">
         <v>17</v>
       </c>
       <c r="O22" s="5" t="s">
@@ -2288,7 +2378,7 @@
       <c r="R22" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="S22" s="6" t="s">
+      <c r="S22" s="15" t="s">
         <v>14</v>
       </c>
       <c r="T22" s="5" t="s">
@@ -2643,13 +2733,13 @@
       <c r="C27" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="F27" s="7" t="s">
         <v>18</v>
       </c>
       <c r="G27" s="6" t="s">
@@ -2889,10 +2979,10 @@
       <c r="E30" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F30" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G30" s="6" t="s">
+      <c r="F30" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" s="11" t="s">
         <v>14</v>
       </c>
       <c r="H30" s="3" t="s">

</xml_diff>